<commit_message>
integrated Bouncy block, visually there but physics unconfirmed
</commit_message>
<xml_diff>
--- a/resources/level_layout.xlsx
+++ b/resources/level_layout.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carri\Desktop\CS308\game_clh87\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6536FEA3-8E85-4D5D-8418-FAB3D9415299}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EF160A-ABB2-4B4A-BF58-8BA1CB65D9A0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7490" xr2:uid="{E620CE8A-FE03-4A0C-B31E-3B7530D0CC5D}"/>
   </bookViews>
@@ -41,7 +41,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,6 +102,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -115,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -131,6 +137,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2E03180-95FA-4203-97F7-A2A72A597E5E}">
   <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" zoomScale="53" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -468,36 +475,6 @@
       <c r="J1" s="1">
         <v>9</v>
       </c>
-      <c r="M1" s="1">
-        <v>10</v>
-      </c>
-      <c r="N1" s="14">
-        <v>11</v>
-      </c>
-      <c r="O1" s="1">
-        <v>12</v>
-      </c>
-      <c r="P1" s="3">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>14</v>
-      </c>
-      <c r="R1" s="1">
-        <v>15</v>
-      </c>
-      <c r="S1" s="3">
-        <v>16</v>
-      </c>
-      <c r="T1" s="1">
-        <v>17</v>
-      </c>
-      <c r="U1" s="14">
-        <v>18</v>
-      </c>
-      <c r="V1" s="1">
-        <v>19</v>
-      </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
@@ -530,35 +507,35 @@
       <c r="J2" s="5">
         <v>19</v>
       </c>
-      <c r="M2" s="14">
-        <v>20</v>
-      </c>
-      <c r="N2" s="1">
-        <v>21</v>
-      </c>
-      <c r="O2" s="3">
-        <v>22</v>
-      </c>
-      <c r="P2" s="1">
-        <v>23</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>24</v>
-      </c>
-      <c r="R2" s="2">
-        <v>25</v>
-      </c>
-      <c r="S2" s="1">
-        <v>26</v>
-      </c>
-      <c r="T2" s="3">
-        <v>27</v>
-      </c>
-      <c r="U2" s="1">
-        <v>28</v>
-      </c>
-      <c r="V2" s="14">
-        <v>29</v>
+      <c r="M2" s="1">
+        <v>10</v>
+      </c>
+      <c r="N2" s="14">
+        <v>11</v>
+      </c>
+      <c r="O2" s="1">
+        <v>12</v>
+      </c>
+      <c r="P2" s="3">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>14</v>
+      </c>
+      <c r="R2" s="1">
+        <v>15</v>
+      </c>
+      <c r="S2" s="3">
+        <v>16</v>
+      </c>
+      <c r="T2" s="1">
+        <v>17</v>
+      </c>
+      <c r="U2" s="14">
+        <v>18</v>
+      </c>
+      <c r="V2" s="1">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
@@ -592,35 +569,35 @@
       <c r="J3" s="5">
         <v>29</v>
       </c>
-      <c r="M3" s="1">
-        <v>30</v>
-      </c>
-      <c r="N3" s="3">
-        <v>31</v>
-      </c>
-      <c r="O3" s="1">
-        <v>32</v>
-      </c>
-      <c r="P3" s="2">
-        <v>33</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>34</v>
-      </c>
-      <c r="R3" s="1">
-        <v>35</v>
-      </c>
-      <c r="S3" s="2">
-        <v>36</v>
-      </c>
-      <c r="T3" s="1">
-        <v>37</v>
-      </c>
-      <c r="U3" s="3">
-        <v>38</v>
-      </c>
-      <c r="V3" s="1">
-        <v>39</v>
+      <c r="M3" s="14">
+        <v>20</v>
+      </c>
+      <c r="N3" s="1">
+        <v>21</v>
+      </c>
+      <c r="O3" s="3">
+        <v>22</v>
+      </c>
+      <c r="P3" s="1">
+        <v>23</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>24</v>
+      </c>
+      <c r="R3" s="2">
+        <v>25</v>
+      </c>
+      <c r="S3" s="1">
+        <v>26</v>
+      </c>
+      <c r="T3" s="3">
+        <v>27</v>
+      </c>
+      <c r="U3" s="1">
+        <v>28</v>
+      </c>
+      <c r="V3" s="14">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
@@ -654,35 +631,35 @@
       <c r="J4" s="5">
         <v>39</v>
       </c>
-      <c r="M4" s="3">
-        <v>40</v>
-      </c>
-      <c r="N4" s="1">
-        <v>41</v>
-      </c>
-      <c r="O4" s="2">
-        <v>42</v>
-      </c>
-      <c r="P4" s="1">
-        <v>43</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>44</v>
-      </c>
-      <c r="R4" s="5">
-        <v>45</v>
-      </c>
-      <c r="S4" s="1">
-        <v>46</v>
-      </c>
-      <c r="T4" s="2">
-        <v>47</v>
-      </c>
-      <c r="U4" s="1">
-        <v>48</v>
-      </c>
-      <c r="V4" s="3">
-        <v>49</v>
+      <c r="M4" s="1">
+        <v>30</v>
+      </c>
+      <c r="N4" s="3">
+        <v>31</v>
+      </c>
+      <c r="O4" s="1">
+        <v>32</v>
+      </c>
+      <c r="P4" s="2">
+        <v>33</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>34</v>
+      </c>
+      <c r="R4" s="1">
+        <v>35</v>
+      </c>
+      <c r="S4" s="2">
+        <v>36</v>
+      </c>
+      <c r="T4" s="1">
+        <v>37</v>
+      </c>
+      <c r="U4" s="3">
+        <v>38</v>
+      </c>
+      <c r="V4" s="1">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
@@ -716,23 +693,35 @@
       <c r="J5" s="1">
         <v>49</v>
       </c>
-      <c r="M5" s="1">
-        <v>50</v>
-      </c>
-      <c r="N5" s="2"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="5">
-        <v>53</v>
-      </c>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="5">
-        <v>56</v>
-      </c>
-      <c r="T5" s="1"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="1">
-        <v>59</v>
+      <c r="M5" s="3">
+        <v>40</v>
+      </c>
+      <c r="N5" s="1">
+        <v>41</v>
+      </c>
+      <c r="O5" s="2">
+        <v>42</v>
+      </c>
+      <c r="P5" s="1">
+        <v>43</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>44</v>
+      </c>
+      <c r="R5" s="5">
+        <v>45</v>
+      </c>
+      <c r="S5" s="1">
+        <v>46</v>
+      </c>
+      <c r="T5" s="2">
+        <v>47</v>
+      </c>
+      <c r="U5" s="1">
+        <v>48</v>
+      </c>
+      <c r="V5" s="3">
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
@@ -750,27 +739,23 @@
       <c r="J6" s="1">
         <v>59</v>
       </c>
-      <c r="M6" s="2">
-        <v>60</v>
-      </c>
-      <c r="N6" s="1"/>
-      <c r="O6" s="5">
-        <v>62</v>
-      </c>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="4">
-        <v>64</v>
-      </c>
-      <c r="R6" s="4">
-        <v>65</v>
-      </c>
-      <c r="S6" s="1"/>
-      <c r="T6" s="5">
-        <v>67</v>
-      </c>
-      <c r="U6" s="1"/>
-      <c r="V6" s="2">
-        <v>69</v>
+      <c r="M6" s="1">
+        <v>50</v>
+      </c>
+      <c r="N6" s="2"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="5">
+        <v>53</v>
+      </c>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="5">
+        <v>56</v>
+      </c>
+      <c r="T6" s="1"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="1">
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
@@ -788,31 +773,27 @@
       <c r="J7" s="1">
         <v>69</v>
       </c>
-      <c r="M7" s="1">
-        <v>70</v>
-      </c>
-      <c r="N7" s="5">
-        <v>71</v>
-      </c>
-      <c r="O7" s="1">
-        <v>72</v>
-      </c>
-      <c r="P7" s="4">
-        <v>73</v>
-      </c>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="4">
-        <v>76</v>
-      </c>
-      <c r="T7" s="1">
-        <v>77</v>
-      </c>
-      <c r="U7" s="5">
-        <v>78</v>
-      </c>
-      <c r="V7" s="1">
-        <v>79</v>
+      <c r="M7" s="2">
+        <v>60</v>
+      </c>
+      <c r="N7" s="1"/>
+      <c r="O7" s="5">
+        <v>62</v>
+      </c>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="4">
+        <v>64</v>
+      </c>
+      <c r="R7" s="4">
+        <v>65</v>
+      </c>
+      <c r="S7" s="1"/>
+      <c r="T7" s="5">
+        <v>67</v>
+      </c>
+      <c r="U7" s="1"/>
+      <c r="V7" s="2">
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.35">
@@ -835,30 +816,30 @@
         <v>79</v>
       </c>
       <c r="M8" s="1">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="N8" s="5">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="O8" s="1">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="P8" s="4">
-        <v>83</v>
-      </c>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
+        <v>73</v>
+      </c>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
       <c r="S8" s="4">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="T8" s="1">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="U8" s="5">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="V8" s="1">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
@@ -881,30 +862,30 @@
         <v>89</v>
       </c>
       <c r="M9" s="1">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="N9" s="5">
-        <v>91</v>
-      </c>
-      <c r="O9" s="11">
-        <v>92</v>
-      </c>
-      <c r="P9" s="8">
-        <v>93</v>
-      </c>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="8">
-        <v>96</v>
-      </c>
-      <c r="T9" s="11">
-        <v>97</v>
+        <v>81</v>
+      </c>
+      <c r="O9" s="1">
+        <v>82</v>
+      </c>
+      <c r="P9" s="4">
+        <v>83</v>
+      </c>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="4">
+        <v>86</v>
+      </c>
+      <c r="T9" s="1">
+        <v>87</v>
       </c>
       <c r="U9" s="5">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="V9" s="1">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.35">
@@ -927,30 +908,30 @@
         <v>99</v>
       </c>
       <c r="M10" s="1">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="N10" s="5">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="O10" s="11">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P10" s="8">
-        <v>103</v>
-      </c>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
+        <v>93</v>
+      </c>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
       <c r="S10" s="8">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="T10" s="11">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="U10" s="5">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="V10" s="1">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.35">
@@ -972,31 +953,31 @@
       <c r="J11" s="1">
         <v>109</v>
       </c>
-      <c r="M11" s="2">
-        <v>110</v>
-      </c>
-      <c r="N11" s="1"/>
-      <c r="O11" s="5">
-        <v>112</v>
-      </c>
-      <c r="P11" s="1">
-        <v>113</v>
-      </c>
-      <c r="Q11" s="4">
-        <v>114</v>
-      </c>
-      <c r="R11" s="4">
-        <v>115</v>
-      </c>
-      <c r="S11" s="1">
-        <v>116</v>
-      </c>
-      <c r="T11" s="5">
-        <v>117</v>
-      </c>
-      <c r="U11" s="1"/>
-      <c r="V11" s="2">
-        <v>119</v>
+      <c r="M11" s="1">
+        <v>100</v>
+      </c>
+      <c r="N11" s="5">
+        <v>101</v>
+      </c>
+      <c r="O11" s="11">
+        <v>102</v>
+      </c>
+      <c r="P11" s="8">
+        <v>103</v>
+      </c>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="8">
+        <v>106</v>
+      </c>
+      <c r="T11" s="11">
+        <v>107</v>
+      </c>
+      <c r="U11" s="5">
+        <v>108</v>
+      </c>
+      <c r="V11" s="1">
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.35">
@@ -1018,27 +999,31 @@
       <c r="J12" s="1">
         <v>119</v>
       </c>
-      <c r="M12" s="1">
-        <v>120</v>
-      </c>
-      <c r="N12" s="2">
-        <v>121</v>
-      </c>
-      <c r="O12" s="1"/>
-      <c r="P12" s="5">
-        <v>123</v>
-      </c>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="5">
-        <v>126</v>
-      </c>
-      <c r="T12" s="1"/>
-      <c r="U12" s="2">
-        <v>128</v>
-      </c>
-      <c r="V12" s="1">
-        <v>129</v>
+      <c r="M12" s="2">
+        <v>110</v>
+      </c>
+      <c r="N12" s="1"/>
+      <c r="O12" s="5">
+        <v>112</v>
+      </c>
+      <c r="P12" s="1">
+        <v>113</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>114</v>
+      </c>
+      <c r="R12" s="4">
+        <v>115</v>
+      </c>
+      <c r="S12" s="1">
+        <v>116</v>
+      </c>
+      <c r="T12" s="5">
+        <v>117</v>
+      </c>
+      <c r="U12" s="1"/>
+      <c r="V12" s="2">
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.35">
@@ -1060,27 +1045,27 @@
       <c r="J13" s="1">
         <v>129</v>
       </c>
-      <c r="M13" s="3">
-        <v>130</v>
-      </c>
-      <c r="N13" s="1"/>
-      <c r="O13" s="2">
-        <v>132</v>
-      </c>
-      <c r="P13" s="1">
-        <v>133</v>
-      </c>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="1">
-        <v>136</v>
-      </c>
-      <c r="T13" s="2">
-        <v>137</v>
-      </c>
-      <c r="U13" s="1"/>
-      <c r="V13" s="3">
-        <v>139</v>
+      <c r="M13" s="1">
+        <v>120</v>
+      </c>
+      <c r="N13" s="2">
+        <v>121</v>
+      </c>
+      <c r="O13" s="1"/>
+      <c r="P13" s="5">
+        <v>123</v>
+      </c>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="5">
+        <v>126</v>
+      </c>
+      <c r="T13" s="1"/>
+      <c r="U13" s="2">
+        <v>128</v>
+      </c>
+      <c r="V13" s="1">
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.35">
@@ -1102,27 +1087,27 @@
       <c r="J14" s="1">
         <v>139</v>
       </c>
-      <c r="M14" s="1">
-        <v>140</v>
-      </c>
-      <c r="N14" s="3"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="2">
-        <v>143</v>
-      </c>
-      <c r="Q14" s="1">
-        <v>144</v>
-      </c>
-      <c r="R14" s="1">
-        <v>145</v>
-      </c>
-      <c r="S14" s="2">
-        <v>146</v>
-      </c>
-      <c r="T14" s="1"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="1">
-        <v>149</v>
+      <c r="M14" s="3">
+        <v>130</v>
+      </c>
+      <c r="N14" s="1"/>
+      <c r="O14" s="2">
+        <v>132</v>
+      </c>
+      <c r="P14" s="1">
+        <v>133</v>
+      </c>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="1">
+        <v>136</v>
+      </c>
+      <c r="T14" s="2">
+        <v>137</v>
+      </c>
+      <c r="U14" s="1"/>
+      <c r="V14" s="3">
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.35">
@@ -1144,23 +1129,27 @@
       <c r="J15" s="1">
         <v>149</v>
       </c>
-      <c r="M15" s="14">
-        <v>150</v>
-      </c>
-      <c r="N15" s="1"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="2">
-        <v>154</v>
-      </c>
-      <c r="R15" s="2">
-        <v>155</v>
-      </c>
-      <c r="S15" s="1"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="14">
-        <v>159</v>
+      <c r="M15" s="1">
+        <v>140</v>
+      </c>
+      <c r="N15" s="3"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="2">
+        <v>143</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>144</v>
+      </c>
+      <c r="R15" s="1">
+        <v>145</v>
+      </c>
+      <c r="S15" s="2">
+        <v>146</v>
+      </c>
+      <c r="T15" s="1"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="1">
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.35">
@@ -1182,23 +1171,23 @@
       <c r="J16" s="1">
         <v>159</v>
       </c>
-      <c r="M16" s="1">
-        <v>160</v>
-      </c>
-      <c r="N16" s="14"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="1">
-        <v>164</v>
-      </c>
-      <c r="R16" s="1">
-        <v>165</v>
-      </c>
-      <c r="S16" s="3"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="14"/>
-      <c r="V16" s="1">
-        <v>169</v>
+      <c r="M16" s="14">
+        <v>150</v>
+      </c>
+      <c r="N16" s="1"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="2">
+        <v>154</v>
+      </c>
+      <c r="R16" s="2">
+        <v>155</v>
+      </c>
+      <c r="S16" s="1"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="14">
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.35">
@@ -1220,88 +1209,110 @@
       <c r="J17" s="1">
         <v>169</v>
       </c>
-      <c r="M17" s="2">
+      <c r="M17" s="1">
+        <v>160</v>
+      </c>
+      <c r="N17" s="14"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="1">
+        <v>164</v>
+      </c>
+      <c r="R17" s="1">
+        <v>165</v>
+      </c>
+      <c r="S17" s="3"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="14"/>
+      <c r="V17" s="1">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A18" s="15">
         <v>170</v>
       </c>
-      <c r="N17" s="1"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="3">
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15">
         <v>174</v>
       </c>
-      <c r="R17" s="3">
+      <c r="F18" s="15">
         <v>175</v>
       </c>
-      <c r="S17" s="1"/>
-      <c r="T17" s="14"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="2">
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15">
         <v>179</v>
       </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A18" s="1">
+      <c r="M18" s="15">
         <v>170</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="5">
+      <c r="N18" s="15"/>
+      <c r="O18" s="15">
+        <v>172</v>
+      </c>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15">
         <v>174</v>
       </c>
-      <c r="F18" s="5">
+      <c r="R18" s="15">
         <v>175</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1">
+      <c r="S18" s="15"/>
+      <c r="T18" s="15">
+        <v>177</v>
+      </c>
+      <c r="U18" s="15"/>
+      <c r="V18" s="15">
         <v>179</v>
       </c>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="15"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>